<commit_message>
optimalize code, change database to mysql
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -18,10 +18,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
-    <t>{1 2018-11-12 13:56:41.745231281 +0800 +0800 2018-11-15 11:56:47.989567114 +0800 +0800 &lt;nil&gt;}</t>
-  </si>
-  <si>
-    <t>100</t>
+    <t>{1 2018-11-15 16:26:10 +0800 CST 2018-11-15 16:26:10 +0800 CST &lt;nil&gt;}</t>
+  </si>
+  <si>
+    <t>553.5</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>wabuguan</t>
+  </si>
+  <si>
+    <t>online</t>
+  </si>
+  <si>
+    <t>abc.txt</t>
+  </si>
+  <si>
+    <t>{2 2018-11-15 16:26:51 +0800 CST 2018-11-15 16:34:44 +0800 CST &lt;nil&gt;}</t>
+  </si>
+  <si>
+    <t>66.14</t>
   </si>
   <si>
     <t>1</t>
@@ -30,16 +48,16 @@
     <t>Alice</t>
   </si>
   <si>
-    <t>online</t>
+    <t>offline</t>
   </si>
   <si>
     <t>image.jpg</t>
   </si>
   <si>
-    <t>{2 2018-11-12 13:57:39.371906946 +0800 +0800 2018-11-12 13:57:39.371906946 +0800 +0800 &lt;nil&gt;}</t>
-  </si>
-  <si>
-    <t>21.12</t>
+    <t>{3 2018-11-15 16:27:35 +0800 CST 2018-11-15 16:27:35 +0800 CST &lt;nil&gt;}</t>
+  </si>
+  <si>
+    <t>43.24</t>
   </si>
   <si>
     <t>2</t>
@@ -48,55 +66,37 @@
     <t>Bob</t>
   </si>
   <si>
-    <t>offline</t>
-  </si>
-  <si>
-    <t>~Bob_file.csv</t>
-  </si>
-  <si>
-    <t>{3 2018-11-12 13:58:27.557820753 +0800 +0800 2018-11-12 13:58:27.557820753 +0800 +0800 &lt;nil&gt;}</t>
-  </si>
-  <si>
-    <t>36.32</t>
+    <t>bob.xlxs</t>
+  </si>
+  <si>
+    <t>{4 2018-11-15 16:28:13 +0800 CST 2018-11-15 16:28:13 +0800 CST &lt;nil&gt;}</t>
+  </si>
+  <si>
+    <t>99.66</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>Calvein</t>
-  </si>
-  <si>
-    <t>~Calvein_file.csv</t>
-  </si>
-  <si>
-    <t>{5 2018-11-12 14:00:02.455299938 +0800 +0800 2018-11-12 14:00:02.455299938 +0800 +0800 &lt;nil&gt;}</t>
-  </si>
-  <si>
-    <t>58.75</t>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>cat.png</t>
+  </si>
+  <si>
+    <t>{17 2018-11-15 17:57:14 +0800 CST 2018-11-15 17:57:14 +0800 CST &lt;nil&gt;}</t>
+  </si>
+  <si>
+    <t>95.2</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>Elvin</t>
-  </si>
-  <si>
-    <t>~Elvin_file.jpg</t>
-  </si>
-  <si>
-    <t>{6 2018-11-12 15:23:12.322685756 +0800 +0800 2018-11-12 15:25:45.935540664 +0800 +0800 &lt;nil&gt;}</t>
-  </si>
-  <si>
-    <t>553.5</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>wabuguan</t>
-  </si>
-  <si>
-    <t>abc.txt</t>
+    <t>Elevant</t>
+  </si>
+  <si>
+    <t>Elevant.png</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>16</v>

</xml_diff>